<commit_message>
Testes entregues na terça
</commit_message>
<xml_diff>
--- a/Testes com Utilizadores.xlsx
+++ b/Testes com Utilizadores.xlsx
@@ -198,10 +198,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Folha1!$A$3:$A$9</c:f>
+              <c:f>Folha1!$A$3:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -222,16 +222,40 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Folha1!$B$3:$B$9</c:f>
+              <c:f>Folha1!$B$3:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>2.0</c:v>
                 </c:pt>
@@ -252,6 +276,30 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -266,11 +314,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2102312960"/>
-        <c:axId val="2102322864"/>
+        <c:axId val="2144279280"/>
+        <c:axId val="2144733616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2102312960"/>
+        <c:axId val="2144279280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -335,12 +383,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2102322864"/>
+        <c:crossAx val="2144733616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2102322864"/>
+        <c:axId val="2144733616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -405,7 +453,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2102312960"/>
+        <c:crossAx val="2144279280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -545,10 +593,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Folha1!$A$3:$A$9</c:f>
+              <c:f>Folha1!$A$3:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -569,16 +617,40 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Folha1!$C$3:$C$9</c:f>
+              <c:f>Folha1!$C$3:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>43.0</c:v>
                 </c:pt>
@@ -599,6 +671,30 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>94.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>69.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>35.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -613,11 +709,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2101587520"/>
-        <c:axId val="2101583872"/>
+        <c:axId val="2112053088"/>
+        <c:axId val="2110434256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2101587520"/>
+        <c:axId val="2112053088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -682,12 +778,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2101583872"/>
+        <c:crossAx val="2110434256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2101583872"/>
+        <c:axId val="2110434256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -752,7 +848,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2101587520"/>
+        <c:crossAx val="2112053088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -890,10 +986,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Folha1!$A$3:$A$9</c:f>
+              <c:f>Folha1!$A$3:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -914,16 +1010,40 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Folha1!$D$3:$D$9</c:f>
+              <c:f>Folha1!$D$3:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>5.0</c:v>
                 </c:pt>
@@ -944,6 +1064,30 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -958,11 +1102,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2099359648"/>
-        <c:axId val="2099356352"/>
+        <c:axId val="2099926016"/>
+        <c:axId val="2102883792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2099359648"/>
+        <c:axId val="2099926016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1019,12 +1163,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2099356352"/>
+        <c:crossAx val="2102883792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2099356352"/>
+        <c:axId val="2102883792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1081,7 +1225,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2099359648"/>
+        <c:crossAx val="2099926016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1221,10 +1365,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Folha1!$A$3:$A$9</c:f>
+              <c:f>Folha1!$A$3:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -1245,16 +1389,40 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Folha1!$F$3:$F$9</c:f>
+              <c:f>Folha1!$F$3:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>2.0</c:v>
                 </c:pt>
@@ -1275,6 +1443,30 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1289,11 +1481,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2099294368"/>
-        <c:axId val="2099290720"/>
+        <c:axId val="2112771200"/>
+        <c:axId val="2112618512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2099294368"/>
+        <c:axId val="2112771200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1358,12 +1550,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2099290720"/>
+        <c:crossAx val="2112618512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2099290720"/>
+        <c:axId val="2112618512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1428,7 +1620,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2099294368"/>
+        <c:crossAx val="2112771200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1568,10 +1760,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Folha1!$A$3:$A$9</c:f>
+              <c:f>Folha1!$A$3:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -1592,16 +1784,40 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Folha1!$G$3:$G$9</c:f>
+              <c:f>Folha1!$G$3:$G$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>45.0</c:v>
                 </c:pt>
@@ -1622,6 +1838,30 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>63.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>34.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1636,11 +1876,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2099260800"/>
-        <c:axId val="2099257152"/>
+        <c:axId val="2108303760"/>
+        <c:axId val="2144070256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2099260800"/>
+        <c:axId val="2108303760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1705,12 +1945,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2099257152"/>
+        <c:crossAx val="2144070256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2099257152"/>
+        <c:axId val="2144070256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1775,7 +2015,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2099260800"/>
+        <c:crossAx val="2108303760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1913,10 +2153,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Folha1!$A$3:$A$9</c:f>
+              <c:f>Folha1!$A$3:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -1937,16 +2177,40 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Folha1!$H$3:$H$9</c:f>
+              <c:f>Folha1!$H$3:$H$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>5.0</c:v>
                 </c:pt>
@@ -1967,6 +2231,30 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1981,11 +2269,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2102738944"/>
-        <c:axId val="2102742240"/>
+        <c:axId val="2139680960"/>
+        <c:axId val="2142341168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2102738944"/>
+        <c:axId val="2139680960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2042,12 +2330,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2102742240"/>
+        <c:crossAx val="2142341168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2102742240"/>
+        <c:axId val="2142341168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2104,7 +2392,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2102738944"/>
+        <c:crossAx val="2139680960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2244,10 +2532,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Folha1!$A$3:$A$9</c:f>
+              <c:f>Folha1!$A$3:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -2268,16 +2556,40 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Folha1!$J$3:$J$9</c:f>
+              <c:f>Folha1!$J$3:$J$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -2297,6 +2609,30 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2312,11 +2648,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2102770848"/>
-        <c:axId val="2102774496"/>
+        <c:axId val="2141668944"/>
+        <c:axId val="2141453280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2102770848"/>
+        <c:axId val="2141668944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2381,12 +2717,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2102774496"/>
+        <c:crossAx val="2141453280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2102774496"/>
+        <c:axId val="2141453280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2451,7 +2787,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2102770848"/>
+        <c:crossAx val="2141668944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2591,10 +2927,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Folha1!$A$3:$A$9</c:f>
+              <c:f>Folha1!$A$3:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -2615,16 +2951,40 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Folha1!$K$3:$K$9</c:f>
+              <c:f>Folha1!$K$3:$K$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>9.0</c:v>
                 </c:pt>
@@ -2645,6 +3005,30 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2659,11 +3043,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2102801872"/>
-        <c:axId val="2102805520"/>
+        <c:axId val="2141916416"/>
+        <c:axId val="2112856272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2102801872"/>
+        <c:axId val="2141916416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2728,12 +3112,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2102805520"/>
+        <c:crossAx val="2112856272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2102805520"/>
+        <c:axId val="2112856272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2798,7 +3182,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2102801872"/>
+        <c:crossAx val="2141916416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2936,10 +3320,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Folha1!$A$3:$A$9</c:f>
+              <c:f>Folha1!$A$3:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -2960,16 +3344,40 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Folha1!$L$3:$L$9</c:f>
+              <c:f>Folha1!$L$3:$L$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>5.0</c:v>
                 </c:pt>
@@ -2989,6 +3397,30 @@
                   <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>5.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3004,11 +3436,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2102833136"/>
-        <c:axId val="2102836432"/>
+        <c:axId val="2141996128"/>
+        <c:axId val="2142554272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2102833136"/>
+        <c:axId val="2141996128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3065,12 +3497,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2102836432"/>
+        <c:crossAx val="2142554272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2102836432"/>
+        <c:axId val="2142554272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3127,7 +3559,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2102833136"/>
+        <c:crossAx val="2141996128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8756,11 +9188,14 @@
   </sheetPr>
   <dimension ref="A1:AB52"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="28" max="28" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
@@ -9094,31 +9529,193 @@
       <c r="A12">
         <v>10</v>
       </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>94</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>6</v>
+      </c>
+      <c r="G12">
+        <v>91</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>31</v>
+      </c>
+      <c r="L12">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>41</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>56</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>12</v>
+      </c>
+      <c r="L13">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>52</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>63</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>11</v>
+      </c>
+      <c r="L14">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>69</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>46</v>
+      </c>
+      <c r="H15">
+        <v>5</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>8</v>
+      </c>
+      <c r="L15">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>39</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>37</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>8</v>
+      </c>
+      <c r="L16">
+        <v>5</v>
+      </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>35</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <v>34</v>
+      </c>
+      <c r="H17">
+        <v>5</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>9</v>
+      </c>
+      <c r="L17">
+        <v>5</v>
+      </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="G22" t="s">
@@ -9126,21 +9723,21 @@
       </c>
       <c r="H22">
         <f>AVERAGE(B3:B17)</f>
-        <v>2.8888888888888888</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="Q22" t="s">
         <v>3</v>
       </c>
       <c r="R22">
         <f>AVERAGE(F3:F17)</f>
-        <v>2.8888888888888888</v>
+        <v>2.4666666666666668</v>
       </c>
       <c r="AA22" t="s">
         <v>3</v>
       </c>
       <c r="AB22">
         <f>AVERAGE(J3:J17)</f>
-        <v>0.1111111111111111</v>
+        <v>6.6666666666666666E-2</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.2">
@@ -9149,21 +9746,21 @@
       </c>
       <c r="H23">
         <f>_xlfn.STDEV.P(B3:B17)</f>
-        <v>1.4487116456005886</v>
+        <v>1.6</v>
       </c>
       <c r="Q23" t="s">
         <v>4</v>
       </c>
       <c r="R23">
         <f>_xlfn.STDEV.P(F3:F17)</f>
-        <v>0.99380798999990649</v>
+        <v>1.586050300449376</v>
       </c>
       <c r="AA23" t="s">
         <v>4</v>
       </c>
       <c r="AB23">
         <f>_xlfn.STDEV.P(J3:J17)</f>
-        <v>0.31426968052735443</v>
+        <v>0.24944382578492943</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
@@ -9172,21 +9769,21 @@
       </c>
       <c r="H24">
         <f>_xlfn.CONFIDENCE.T(0.05,H23,15)</f>
-        <v>0.8022697683836707</v>
+        <v>0.88605046650378883</v>
       </c>
       <c r="Q24" t="s">
         <v>5</v>
       </c>
       <c r="R24">
         <f>_xlfn.CONFIDENCE.T(0.05,R23,15)</f>
-        <v>0.5503525207216311</v>
+        <v>0.87832538038227759</v>
       </c>
       <c r="AA24" t="s">
         <v>5</v>
       </c>
       <c r="AB24">
         <f>_xlfn.CONFIDENCE.T(0.05,AB23,15)</f>
-        <v>0.17403674814953693</v>
+        <v>0.13813738637701661</v>
       </c>
     </row>
     <row r="37" spans="7:28" x14ac:dyDescent="0.2">
@@ -9194,22 +9791,22 @@
         <v>3</v>
       </c>
       <c r="H37">
-        <f>AVERAGE(C3:C17)</f>
-        <v>38.777777777777779</v>
+        <f>AVERAGE(C13:C17,C3:C11)</f>
+        <v>41.785714285714285</v>
       </c>
       <c r="Q37" t="s">
         <v>3</v>
       </c>
       <c r="R37">
-        <f>AVERAGE(G3:G17)</f>
-        <v>34</v>
+        <f>AVERAGE(G3:G11,G13:G15)</f>
+        <v>39.25</v>
       </c>
       <c r="AA37" t="s">
         <v>3</v>
       </c>
       <c r="AB37">
-        <f>AVERAGE(K3:K17)</f>
-        <v>11.111111111111111</v>
+        <f>AVERAGE(K3:K11,K13:K17)</f>
+        <v>10.571428571428571</v>
       </c>
     </row>
     <row r="38" spans="7:28" x14ac:dyDescent="0.2">
@@ -9217,22 +9814,22 @@
         <v>4</v>
       </c>
       <c r="H38">
-        <f>_xlfn.STDEV.P(C3:C17)</f>
-        <v>8.5735740994935234</v>
+        <f>_xlfn.STDEV.P(C3:C11,C13:C17)</f>
+        <v>10.831030629159716</v>
       </c>
       <c r="Q38" t="s">
         <v>4</v>
       </c>
       <c r="R38">
-        <f>_xlfn.STDEV.P(G3:G17)</f>
-        <v>7.333333333333333</v>
+        <f>_xlfn.STDEV.P(G3:G11,G13:G17)</f>
+        <v>10.859022393702794</v>
       </c>
       <c r="AA38" t="s">
         <v>4</v>
       </c>
       <c r="AB38">
-        <f>_xlfn.STDEV.P(K3:K17)</f>
-        <v>3.5728744868474505</v>
+        <f>_xlfn.STDEV.P(K3:K11,K13:K17)</f>
+        <v>3.1102201510110343</v>
       </c>
     </row>
     <row r="39" spans="7:28" x14ac:dyDescent="0.2">
@@ -9240,22 +9837,22 @@
         <v>5</v>
       </c>
       <c r="H39">
-        <f>_xlfn.CONFIDENCE.T(0.05,H38,15)</f>
-        <v>4.7478870815381491</v>
+        <f>_xlfn.CONFIDENCE.T(0.05,H38,14)</f>
+        <v>6.2536509011050256</v>
       </c>
       <c r="Q39" t="s">
         <v>5</v>
       </c>
       <c r="R39">
-        <f>_xlfn.CONFIDENCE.T(0.05,R38,15)</f>
-        <v>4.0610646381423656</v>
+        <f>_xlfn.CONFIDENCE.T(0.05,R38,14)</f>
+        <v>6.2698128647769824</v>
       </c>
       <c r="AA39" t="s">
         <v>5</v>
       </c>
       <c r="AB39">
-        <f>_xlfn.CONFIDENCE.T(0.05,AB38,15)</f>
-        <v>1.9785919411441679</v>
+        <f>_xlfn.CONFIDENCE.T(0.05,AB38,14)</f>
+        <v>1.7957876508668071</v>
       </c>
     </row>
     <row r="50" spans="7:28" x14ac:dyDescent="0.2">
@@ -9264,14 +9861,14 @@
       </c>
       <c r="H50">
         <f>AVERAGE(D3:D17)</f>
-        <v>4.7777777777777777</v>
+        <v>4.7333333333333334</v>
       </c>
       <c r="Q50" t="s">
         <v>3</v>
       </c>
       <c r="R50">
         <f>AVERAGE(H3:H17)</f>
-        <v>4.666666666666667</v>
+        <v>4.4666666666666668</v>
       </c>
       <c r="AA50" t="s">
         <v>3</v>
@@ -9287,14 +9884,14 @@
       </c>
       <c r="H51">
         <f>_xlfn.STDEV.P(D3:D17)</f>
-        <v>0.41573970964154905</v>
+        <v>0.44221663871405331</v>
       </c>
       <c r="Q51" t="s">
         <v>4</v>
       </c>
       <c r="R51">
         <f>_xlfn.STDEV.P(H3:H17)</f>
-        <v>0.66666666666666663</v>
+        <v>0.71802197428460057</v>
       </c>
       <c r="AA51" t="s">
         <v>4</v>
@@ -9310,21 +9907,20 @@
       </c>
       <c r="H52">
         <f>_xlfn.CONFIDENCE.T(0.05,H51,15)</f>
-        <v>0.23022897729502764</v>
+        <v>0.24489141189270275</v>
       </c>
       <c r="Q52" t="s">
         <v>5</v>
       </c>
       <c r="R52">
         <f>_xlfn.CONFIDENCE.T(0.05,R51,15)</f>
-        <v>0.36918769437657861</v>
+        <v>0.39762731579677613</v>
       </c>
       <c r="AA52" t="s">
         <v>5</v>
       </c>
-      <c r="AB52" t="e">
-        <f>_xlfn.CONFIDENCE.T(0.05,AB51,15)</f>
-        <v>#NUM!</v>
+      <c r="AB52">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>